<commit_message>
added new testcase TC_InvalidLogin
</commit_message>
<xml_diff>
--- a/Testdata.xlsx
+++ b/Testdata.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Eclipse2\Selenium_Framework_Practice1\"/>
     </mc:Choice>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>country</t>
   </si>
@@ -68,6 +68,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -388,35 +389,35 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>11</v>
       </c>
     </row>
@@ -436,18 +437,18 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>6</v>
       </c>
     </row>

</xml_diff>